<commit_message>
updated 2 excel inserted
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/example.xlsx
+++ b/src/main/java/org/example/example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibattula\IdeaProjects\TyageshProject\src\main\java\org\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ReadWriteXl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFB0846-89FA-4FD2-80BF-4258FCD4D267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471F1FB5-D761-452A-A310-8366BF8DC16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -668,7 +668,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15669" uniqueCount="2238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15664" uniqueCount="2285">
   <si>
     <t>Record Type</t>
   </si>
@@ -7583,6 +7583,147 @@
   </si>
   <si>
     <t>Flag</t>
+  </si>
+  <si>
+    <t>Plan Eff Date</t>
+  </si>
+  <si>
+    <t>Plan Term Date</t>
+  </si>
+  <si>
+    <t>Plan Name</t>
+  </si>
+  <si>
+    <t>Plan Eligibility Override</t>
+  </si>
+  <si>
+    <t>Plan Verify Member</t>
+  </si>
+  <si>
+    <t>Plan Customer Location</t>
+  </si>
+  <si>
+    <t>Plan Verify RX Network</t>
+  </si>
+  <si>
+    <t>Plan Verify Care Facility</t>
+  </si>
+  <si>
+    <t>Plan Verify MD Network</t>
+  </si>
+  <si>
+    <t>Plan DEA Validation</t>
+  </si>
+  <si>
+    <t>Plan Verify MD Specialty</t>
+  </si>
+  <si>
+    <t>Plan Verify Compound</t>
+  </si>
+  <si>
+    <t>Plan Verify NDC List</t>
+  </si>
+  <si>
+    <t>Plan Verify GPI List</t>
+  </si>
+  <si>
+    <t>Plan Verify Maint Drug</t>
+  </si>
+  <si>
+    <t>Plan Verify DEA Code</t>
+  </si>
+  <si>
+    <t>Days Supply/Qty Disp Lmts</t>
+  </si>
+  <si>
+    <t>Plan Verify Refill Limits</t>
+  </si>
+  <si>
+    <t>Plan Verify Legend OTC</t>
+  </si>
+  <si>
+    <t>Plan Verify 3rd Pty Excp</t>
+  </si>
+  <si>
+    <t>Plan Verify Route of Admn</t>
+  </si>
+  <si>
+    <t>Plan Verify Dosage Form</t>
+  </si>
+  <si>
+    <t>Plan DESI Indicator</t>
+  </si>
+  <si>
+    <t>Plan Verify Packaging</t>
+  </si>
+  <si>
+    <t>Plan Verify FDA Ther Equi</t>
+  </si>
+  <si>
+    <t>Plan Verify Therapy</t>
+  </si>
+  <si>
+    <t>Plan Verify Brnd/Gen Subs</t>
+  </si>
+  <si>
+    <t>Plan Level of Service</t>
+  </si>
+  <si>
+    <t>Plan Preferred Formulary</t>
+  </si>
+  <si>
+    <t>Plan Verify Restrictions</t>
+  </si>
+  <si>
+    <t>Plan Verify Pricing</t>
+  </si>
+  <si>
+    <t>Deductible/Cap Limits</t>
+  </si>
+  <si>
+    <t>Plan Default Drug Status</t>
+  </si>
+  <si>
+    <t>PET Plan Type</t>
+  </si>
+  <si>
+    <t>Plan Qualifier</t>
+  </si>
+  <si>
+    <t>DUG Table Name</t>
+  </si>
+  <si>
+    <t>Plan Pref Prod Schedule</t>
+  </si>
+  <si>
+    <t>Plan Audit Flag</t>
+  </si>
+  <si>
+    <t>Plan Patient Pay Qual</t>
+  </si>
+  <si>
+    <t>Plan Verify Specialty Pgm</t>
+  </si>
+  <si>
+    <t>Plan Verify FormMgmtSrvc</t>
+  </si>
+  <si>
+    <t>Plan Discount Benefit</t>
+  </si>
+  <si>
+    <t>Plan Real-Time PA</t>
+  </si>
+  <si>
+    <t>Plan External Program</t>
+  </si>
+  <si>
+    <t>PE1 PQE Messaging Type</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>PE1 Plan Verify ServiceCd</t>
   </si>
 </sst>
 </file>
@@ -7651,7 +7792,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7691,6 +7832,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7787,7 +7934,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -7969,6 +8116,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8532,10 +8682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854DD289-DBBE-4BA2-B108-457D91ED67DC}">
-  <dimension ref="A1:BA17"/>
+  <dimension ref="A1:BA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8553,10 +8703,10 @@
   <sheetData>
     <row r="1" spans="1:53" ht="32.5" x14ac:dyDescent="0.35">
       <c r="A1" s="13"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13" t="s">
         <v>2237</v>
       </c>
-      <c r="C1" s="13"/>
       <c r="D1" s="33" t="s">
         <v>491</v>
       </c>
@@ -9013,154 +9163,154 @@
       </c>
     </row>
     <row r="4" spans="1:53" ht="32.5" x14ac:dyDescent="0.35">
-      <c r="D4" s="29" t="s">
-        <v>491</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>492</v>
-      </c>
-      <c r="F4" s="29" t="s">
-        <v>493</v>
-      </c>
-      <c r="G4" s="29" t="s">
-        <v>574</v>
-      </c>
-      <c r="H4" s="29" t="s">
-        <v>575</v>
-      </c>
-      <c r="I4" s="29" t="s">
-        <v>576</v>
-      </c>
-      <c r="J4" s="29" t="s">
-        <v>577</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>578</v>
-      </c>
-      <c r="L4" s="29" t="s">
-        <v>579</v>
-      </c>
-      <c r="M4" s="29" t="s">
-        <v>580</v>
-      </c>
-      <c r="N4" s="29" t="s">
-        <v>581</v>
-      </c>
-      <c r="O4" s="29" t="s">
-        <v>582</v>
-      </c>
-      <c r="P4" s="29" t="s">
-        <v>583</v>
-      </c>
-      <c r="Q4" s="29" t="s">
-        <v>584</v>
-      </c>
-      <c r="R4" s="29" t="s">
-        <v>585</v>
-      </c>
-      <c r="S4" s="29" t="s">
-        <v>586</v>
-      </c>
-      <c r="T4" s="29" t="s">
-        <v>587</v>
-      </c>
-      <c r="U4" s="29" t="s">
-        <v>588</v>
-      </c>
-      <c r="V4" s="29" t="s">
-        <v>589</v>
-      </c>
-      <c r="W4" s="29" t="s">
-        <v>590</v>
-      </c>
-      <c r="X4" s="29" t="s">
-        <v>591</v>
-      </c>
-      <c r="Y4" s="29" t="s">
-        <v>592</v>
-      </c>
-      <c r="Z4" s="29" t="s">
-        <v>593</v>
-      </c>
-      <c r="AA4" s="29" t="s">
-        <v>594</v>
-      </c>
-      <c r="AB4" s="29" t="s">
-        <v>595</v>
-      </c>
-      <c r="AC4" s="29" t="s">
-        <v>596</v>
-      </c>
-      <c r="AD4" s="29" t="s">
-        <v>597</v>
-      </c>
-      <c r="AE4" s="29" t="s">
-        <v>598</v>
-      </c>
-      <c r="AF4" s="29" t="s">
-        <v>599</v>
-      </c>
-      <c r="AG4" s="29" t="s">
-        <v>600</v>
-      </c>
-      <c r="AH4" s="29" t="s">
-        <v>601</v>
-      </c>
-      <c r="AI4" s="29" t="s">
-        <v>602</v>
-      </c>
-      <c r="AJ4" s="29" t="s">
-        <v>603</v>
-      </c>
-      <c r="AK4" s="29" t="s">
-        <v>604</v>
-      </c>
-      <c r="AL4" s="29" t="s">
-        <v>605</v>
-      </c>
-      <c r="AM4" s="29" t="s">
-        <v>606</v>
-      </c>
-      <c r="AN4" s="29" t="s">
-        <v>607</v>
-      </c>
-      <c r="AO4" s="29" t="s">
-        <v>608</v>
-      </c>
-      <c r="AP4" s="29" t="s">
-        <v>609</v>
-      </c>
-      <c r="AQ4" s="29" t="s">
-        <v>610</v>
-      </c>
-      <c r="AR4" s="29" t="s">
-        <v>611</v>
-      </c>
-      <c r="AS4" s="29" t="s">
-        <v>612</v>
-      </c>
-      <c r="AT4" s="29" t="s">
-        <v>613</v>
-      </c>
-      <c r="AU4" s="29" t="s">
-        <v>614</v>
-      </c>
-      <c r="AV4" s="29" t="s">
-        <v>615</v>
-      </c>
-      <c r="AW4" s="25" t="s">
-        <v>616</v>
-      </c>
-      <c r="AX4" s="25" t="s">
-        <v>617</v>
-      </c>
-      <c r="AY4" s="25" t="s">
-        <v>618</v>
-      </c>
-      <c r="AZ4" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="BA4" s="25" t="s">
+      <c r="D4" s="69" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="69" t="s">
+        <v>2238</v>
+      </c>
+      <c r="F4" s="69" t="s">
+        <v>2239</v>
+      </c>
+      <c r="G4" s="69" t="s">
+        <v>2240</v>
+      </c>
+      <c r="H4" s="69" t="s">
+        <v>2241</v>
+      </c>
+      <c r="I4" s="69" t="s">
+        <v>2242</v>
+      </c>
+      <c r="J4" s="69" t="s">
+        <v>2243</v>
+      </c>
+      <c r="K4" s="69" t="s">
+        <v>2244</v>
+      </c>
+      <c r="L4" s="69" t="s">
+        <v>2245</v>
+      </c>
+      <c r="M4" s="69" t="s">
+        <v>2246</v>
+      </c>
+      <c r="N4" s="69" t="s">
+        <v>2247</v>
+      </c>
+      <c r="O4" s="69" t="s">
+        <v>2248</v>
+      </c>
+      <c r="P4" s="69" t="s">
+        <v>2249</v>
+      </c>
+      <c r="Q4" s="69" t="s">
+        <v>2250</v>
+      </c>
+      <c r="R4" s="69" t="s">
+        <v>2251</v>
+      </c>
+      <c r="S4" s="69" t="s">
+        <v>2252</v>
+      </c>
+      <c r="T4" s="69" t="s">
+        <v>2253</v>
+      </c>
+      <c r="U4" s="69" t="s">
+        <v>2254</v>
+      </c>
+      <c r="V4" s="69" t="s">
+        <v>2255</v>
+      </c>
+      <c r="W4" s="69" t="s">
+        <v>2256</v>
+      </c>
+      <c r="X4" s="69" t="s">
+        <v>2257</v>
+      </c>
+      <c r="Y4" s="69" t="s">
+        <v>2258</v>
+      </c>
+      <c r="Z4" s="69" t="s">
+        <v>2259</v>
+      </c>
+      <c r="AA4" s="69" t="s">
+        <v>2260</v>
+      </c>
+      <c r="AB4" s="69" t="s">
+        <v>2261</v>
+      </c>
+      <c r="AC4" s="69" t="s">
+        <v>2262</v>
+      </c>
+      <c r="AD4" s="69" t="s">
+        <v>2263</v>
+      </c>
+      <c r="AE4" s="69" t="s">
+        <v>2264</v>
+      </c>
+      <c r="AF4" s="69" t="s">
+        <v>2265</v>
+      </c>
+      <c r="AG4" s="69" t="s">
+        <v>2266</v>
+      </c>
+      <c r="AH4" s="69" t="s">
+        <v>2267</v>
+      </c>
+      <c r="AI4" s="69" t="s">
+        <v>2268</v>
+      </c>
+      <c r="AJ4" s="69" t="s">
+        <v>2269</v>
+      </c>
+      <c r="AK4" s="69" t="s">
+        <v>2270</v>
+      </c>
+      <c r="AL4" s="69" t="s">
+        <v>2271</v>
+      </c>
+      <c r="AM4" s="69" t="s">
+        <v>2272</v>
+      </c>
+      <c r="AN4" s="69" t="s">
+        <v>2273</v>
+      </c>
+      <c r="AO4" s="69" t="s">
+        <v>2274</v>
+      </c>
+      <c r="AP4" s="69" t="s">
+        <v>2275</v>
+      </c>
+      <c r="AQ4" s="69" t="s">
+        <v>2276</v>
+      </c>
+      <c r="AR4" s="69" t="s">
+        <v>2277</v>
+      </c>
+      <c r="AS4" s="69" t="s">
+        <v>2278</v>
+      </c>
+      <c r="AT4" s="69" t="s">
+        <v>2279</v>
+      </c>
+      <c r="AU4" s="69" t="s">
+        <v>2280</v>
+      </c>
+      <c r="AV4" s="69" t="s">
+        <v>2281</v>
+      </c>
+      <c r="AW4" s="69" t="s">
+        <v>2282</v>
+      </c>
+      <c r="AX4" s="69" t="s">
+        <v>2283</v>
+      </c>
+      <c r="AY4" s="69" t="s">
+        <v>2283</v>
+      </c>
+      <c r="AZ4" s="69" t="s">
+        <v>2284</v>
+      </c>
+      <c r="BA4" s="30" t="s">
         <v>619</v>
       </c>
     </row>
@@ -10413,26 +10563,6 @@
       <c r="AZ13" s="3"/>
       <c r="BA13" s="3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="C14" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="C15" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.35">
-      <c r="C16" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C17" s="11" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -10441,7 +10571,7 @@
       <formula>LEN($A1) &gt; 25</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4:BA4">
+  <conditionalFormatting sqref="BA4">
     <cfRule type="expression" dxfId="54" priority="1">
       <formula>LEN($A4) &gt; 25</formula>
     </cfRule>
@@ -15076,7 +15206,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15094,9 +15224,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="22" x14ac:dyDescent="0.35">
       <c r="A1" s="13"/>
-      <c r="B1" s="13" t="s">
-        <v>2237</v>
-      </c>
+      <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="33" t="s">
         <v>491</v>

</xml_diff>

<commit_message>
Updated code according to header placement
</commit_message>
<xml_diff>
--- a/src/main/java/org/example/example.xlsx
+++ b/src/main/java/org/example/example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ReadWriteXl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ibattula\IdeaProjects\TyageshProject\src\main\java\org\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471F1FB5-D761-452A-A310-8366BF8DC16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BC45DB-983E-46E1-B271-628C3EF80D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -668,7 +668,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15664" uniqueCount="2285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15665" uniqueCount="2285">
   <si>
     <t>Record Type</t>
   </si>
@@ -8685,7 +8685,7 @@
   <dimension ref="A1:BA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8703,10 +8703,10 @@
   <sheetData>
     <row r="1" spans="1:53" ht="32.5" x14ac:dyDescent="0.35">
       <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13" t="s">
+      <c r="B1" s="13" t="s">
         <v>2237</v>
       </c>
+      <c r="C1" s="13"/>
       <c r="D1" s="33" t="s">
         <v>491</v>
       </c>
@@ -9163,6 +9163,9 @@
       </c>
     </row>
     <row r="4" spans="1:53" ht="32.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="8" t="s">
+        <v>2237</v>
+      </c>
       <c r="D4" s="69" t="s">
         <v>1</v>
       </c>

</xml_diff>